<commit_message>
Version 3, many changes
</commit_message>
<xml_diff>
--- a/board/BOM.xlsx
+++ b/board/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="92">
   <si>
     <t>Qty</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Zener Diode</t>
   </si>
   <si>
-    <t>22pF</t>
-  </si>
-  <si>
     <t>CAPACITOR-2.5MM</t>
   </si>
   <si>
@@ -119,9 +116,6 @@
     <t>D1</t>
   </si>
   <si>
-    <t>470uF</t>
-  </si>
-  <si>
     <t>CAP-POL-25-14</t>
   </si>
   <si>
@@ -140,18 +134,12 @@
     <t>F1</t>
   </si>
   <si>
-    <t>5.1V</t>
-  </si>
-  <si>
     <t>D3</t>
   </si>
   <si>
     <t>R6</t>
   </si>
   <si>
-    <t>8Mhz</t>
-  </si>
-  <si>
     <t>CRYSTAL-V</t>
   </si>
   <si>
@@ -161,12 +149,6 @@
     <t>Crystal Oscillator</t>
   </si>
   <si>
-    <t>ATTINY84-20PU</t>
-  </si>
-  <si>
-    <t>DIP14</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -212,12 +194,6 @@
     <t>DC-DC Converter</t>
   </si>
   <si>
-    <t>SCREW-TERM-5</t>
-  </si>
-  <si>
-    <t>5-Pin Screw Terminal</t>
-  </si>
-  <si>
     <t>FUSE_5X20MM</t>
   </si>
   <si>
@@ -230,30 +206,15 @@
     <t>Ammo pack</t>
   </si>
   <si>
-    <t>EEU-FR1H471B</t>
-  </si>
-  <si>
-    <t>Expensive but long-life</t>
-  </si>
-  <si>
     <t>1N5254B-TAP</t>
   </si>
   <si>
     <t>1N5251B-TAP</t>
   </si>
   <si>
-    <t>FOXSLF/080-20</t>
-  </si>
-  <si>
-    <t>14P</t>
-  </si>
-  <si>
     <t>Socket</t>
   </si>
   <si>
-    <t>1-2199298-3</t>
-  </si>
-  <si>
     <t>BT137-600E,127</t>
   </si>
   <si>
@@ -266,15 +227,6 @@
     <t>MFR-25FBF52-1K</t>
   </si>
   <si>
-    <t>MFR-25FBF52-220R</t>
-  </si>
-  <si>
-    <t>MFR-25FBF52-68R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1N5231B-TAP </t>
-  </si>
-  <si>
     <t>5MT 4-R</t>
   </si>
   <si>
@@ -293,28 +245,61 @@
     <t>4A-MEDIUM-BLOW</t>
   </si>
   <si>
-    <t>SCREW-TERM-6</t>
-  </si>
-  <si>
-    <t>6-Pin Screw Terminal</t>
-  </si>
-  <si>
-    <t>SCREW-TERM-7</t>
-  </si>
-  <si>
-    <t>7-Pin Screw Terminal</t>
-  </si>
-  <si>
     <t>SR151A200JAR</t>
   </si>
   <si>
     <t>K104K15X7RF53L2</t>
   </si>
   <si>
-    <t>Bulk. Need 2.5mm spacing on the board</t>
-  </si>
-  <si>
     <t>FK14X7R1H105K</t>
+  </si>
+  <si>
+    <t>16Mhz</t>
+  </si>
+  <si>
+    <t>ATS16A</t>
+  </si>
+  <si>
+    <t>1-2199298-9</t>
+  </si>
+  <si>
+    <t>DIP28</t>
+  </si>
+  <si>
+    <t>28P</t>
+  </si>
+  <si>
+    <t>ATMEGA328P-PU</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>MF1/4DC68R0F</t>
+  </si>
+  <si>
+    <t>MF1/4DC2200F</t>
+  </si>
+  <si>
+    <t>20pF</t>
+  </si>
+  <si>
+    <t>Expensive but long-life, 470uF version is EEU-FR1H471B</t>
+  </si>
+  <si>
+    <t>EEU-FR1H102</t>
+  </si>
+  <si>
+    <t>1000uF</t>
+  </si>
+  <si>
+    <t>1N5240B-TAP</t>
+  </si>
+  <si>
+    <t>10V</t>
   </si>
 </sst>
 </file>
@@ -358,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -366,6 +351,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,7 +635,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,36 +667,39 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>95</v>
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -718,105 +707,111 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>77</v>
+        <v>58</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>79</v>
-      </c>
-      <c r="H5" t="s">
-        <v>78</v>
+        <v>74</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
       </c>
       <c r="H6" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
-      <c r="B7" s="3">
-        <v>220</v>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -825,91 +820,82 @@
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="H7" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>71</v>
-      </c>
-      <c r="G8" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="H8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>26</v>
+      <c r="B9" s="3">
+        <v>220</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>93</v>
-      </c>
-      <c r="G9" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="H9" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>29</v>
+      <c r="B10" s="3">
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="F10" t="s">
-        <v>70</v>
-      </c>
-      <c r="G10" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="H10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -917,25 +903,25 @@
         <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F11" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="G11" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="H11" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -943,42 +929,51 @@
         <v>1</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F12" t="s">
-        <v>83</v>
+        <v>61</v>
+      </c>
+      <c r="G12" t="s">
+        <v>25</v>
       </c>
       <c r="H12" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>35</v>
+        <v>91</v>
       </c>
       <c r="C13" t="s">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>86</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>87</v>
+        <v>90</v>
+      </c>
+      <c r="G13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -986,48 +981,45 @@
         <v>1</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F14" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="G14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
-      <c r="B15" s="3">
-        <v>68</v>
+      <c r="B15" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F15" t="s">
-        <v>81</v>
-      </c>
-      <c r="H15" t="s">
-        <v>78</v>
+        <v>48</v>
+      </c>
+      <c r="G15" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1035,195 +1027,144 @@
         <v>1</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" t="s">
         <v>41</v>
       </c>
-      <c r="C16" t="s">
+      <c r="F17" t="s">
+        <v>81</v>
+      </c>
+      <c r="G17" t="s">
         <v>42</v>
       </c>
-      <c r="D16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16" t="s">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" t="s">
+        <v>78</v>
+      </c>
+      <c r="H18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" t="s">
+        <v>77</v>
+      </c>
+      <c r="G19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="G16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" t="s">
-        <v>45</v>
-      </c>
-      <c r="G17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" t="s">
-        <v>52</v>
-      </c>
-      <c r="F19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="F20" t="s">
-        <v>54</v>
-      </c>
-      <c r="G20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="H20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="E21" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="F21" t="s">
-        <v>58</v>
-      </c>
-      <c r="G21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" t="s">
-        <v>89</v>
-      </c>
-      <c r="D22" t="s">
-        <v>89</v>
-      </c>
-      <c r="F22" s="3">
-        <v>1935200</v>
-      </c>
-      <c r="G22" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" t="s">
-        <v>62</v>
-      </c>
-      <c r="F23" s="3">
-        <v>1935190</v>
-      </c>
-      <c r="G23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>1</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C24" t="s">
-        <v>91</v>
-      </c>
-      <c r="D24" t="s">
-        <v>91</v>
-      </c>
-      <c r="F24" s="3">
-        <v>1935213</v>
-      </c>
-      <c r="G24" t="s">
-        <v>92</v>
-      </c>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F24" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add soft-start capability to avoid high inrush current
</commit_message>
<xml_diff>
--- a/board/BOM.xlsx
+++ b/board/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="95">
   <si>
     <t>Qty</t>
   </si>
@@ -300,6 +300,15 @@
   </si>
   <si>
     <t>10V</t>
+  </si>
+  <si>
+    <t>MF1/4DC3903F</t>
+  </si>
+  <si>
+    <t>330K</t>
+  </si>
+  <si>
+    <t>R9</t>
   </si>
 </sst>
 </file>
@@ -632,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,7 +739,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>18</v>
@@ -808,10 +817,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -820,10 +829,10 @@
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="F7" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="H7" t="s">
         <v>65</v>
@@ -834,7 +843,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -843,10 +852,10 @@
         <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H8" t="s">
         <v>65</v>
@@ -856,8 +865,8 @@
       <c r="A9">
         <v>2</v>
       </c>
-      <c r="B9" s="3">
-        <v>220</v>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -866,10 +875,10 @@
         <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F9" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="H9" t="s">
         <v>65</v>
@@ -877,10 +886,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" s="3">
-        <v>68</v>
+        <v>220</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -889,10 +898,10 @@
         <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H10" t="s">
         <v>65</v>
@@ -902,26 +911,23 @@
       <c r="A11">
         <v>1</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>28</v>
+      <c r="B11" s="3">
+        <v>68</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="F11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G11" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="H11" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -929,7 +935,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
         <v>22</v>
@@ -938,10 +944,10 @@
         <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G12" t="s">
         <v>25</v>
@@ -955,7 +961,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
         <v>22</v>
@@ -964,10 +970,10 @@
         <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="F13" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="G13" t="s">
         <v>25</v>
@@ -978,25 +984,28 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F14" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="G14" t="s">
-        <v>47</v>
+        <v>25</v>
+      </c>
+      <c r="H14" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1004,45 +1013,45 @@
         <v>1</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D15" t="s">
         <v>45</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="G15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1050,22 +1059,22 @@
         <v>1</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>81</v>
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="E17" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="F17" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="G17" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1073,10 +1082,10 @@
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" t="s">
-        <v>62</v>
+        <v>81</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>81</v>
       </c>
       <c r="D18" t="s">
         <v>79</v>
@@ -1085,10 +1094,10 @@
         <v>41</v>
       </c>
       <c r="F18" t="s">
-        <v>78</v>
-      </c>
-      <c r="H18" t="s">
-        <v>83</v>
+        <v>81</v>
+      </c>
+      <c r="G18" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1096,22 +1105,22 @@
         <v>1</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="E19" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F19" t="s">
-        <v>77</v>
-      </c>
-      <c r="G19" t="s">
-        <v>40</v>
+        <v>78</v>
+      </c>
+      <c r="H19" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1119,52 +1128,75 @@
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F20" t="s">
-        <v>67</v>
-      </c>
-      <c r="H20" t="s">
-        <v>68</v>
+        <v>77</v>
+      </c>
+      <c r="G20" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="E21" t="s">
         <v>35</v>
       </c>
       <c r="F21" t="s">
+        <v>67</v>
+      </c>
+      <c r="H21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F25" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Many changes for version 3
</commit_message>
<xml_diff>
--- a/board/BOM.xlsx
+++ b/board/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="99">
   <si>
     <t>Qty</t>
   </si>
@@ -50,9 +50,6 @@
     <t>CAPACITOR-5MM</t>
   </si>
   <si>
-    <t>C5, C7, C10</t>
-  </si>
-  <si>
     <t>Ceramic Capacitor</t>
   </si>
   <si>
@@ -65,30 +62,15 @@
     <t>AXIAL-7.5MM</t>
   </si>
   <si>
-    <t>R3, R8</t>
-  </si>
-  <si>
     <t>10uF</t>
   </si>
   <si>
-    <t>C1, C3</t>
-  </si>
-  <si>
     <t>1K</t>
   </si>
   <si>
-    <t>R1, R2</t>
-  </si>
-  <si>
     <t>1uF</t>
   </si>
   <si>
-    <t>C6, C8, C9</t>
-  </si>
-  <si>
-    <t>R4, R5</t>
-  </si>
-  <si>
     <t>22V</t>
   </si>
   <si>
@@ -107,9 +89,6 @@
     <t>CAPACITOR-2.5MM</t>
   </si>
   <si>
-    <t>C11, C12</t>
-  </si>
-  <si>
     <t>27V</t>
   </si>
   <si>
@@ -119,9 +98,6 @@
     <t>CAP-POL-25-14</t>
   </si>
   <si>
-    <t>C4</t>
-  </si>
-  <si>
     <t>Polarized Capacitor</t>
   </si>
   <si>
@@ -134,12 +110,6 @@
     <t>F1</t>
   </si>
   <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
     <t>CRYSTAL-V</t>
   </si>
   <si>
@@ -230,9 +200,6 @@
     <t>5MT 4-R</t>
   </si>
   <si>
-    <t>Need to experiement to find appropriate fuse type</t>
-  </si>
-  <si>
     <t>FUSE CLIP</t>
   </si>
   <si>
@@ -302,13 +269,58 @@
     <t>10V</t>
   </si>
   <si>
-    <t>MF1/4DC3903F</t>
-  </si>
-  <si>
-    <t>330K</t>
-  </si>
-  <si>
-    <t>R9</t>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>SUP75P03-07-E3</t>
+  </si>
+  <si>
+    <t>SUP75P03-07-E3-H</t>
+  </si>
+  <si>
+    <t>560K</t>
+  </si>
+  <si>
+    <t>Need to experiment to find appropriate fuse type</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2, R8</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R5, R6</t>
+  </si>
+  <si>
+    <t>R3, R4</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C8, C9</t>
+  </si>
+  <si>
+    <t>C4, C5, C10</t>
+  </si>
+  <si>
+    <t>C1, C2, C7</t>
+  </si>
+  <si>
+    <t>C3, C6</t>
+  </si>
+  <si>
+    <t>D3, D4</t>
+  </si>
+  <si>
+    <t>Bulk (maybe)</t>
+  </si>
+  <si>
+    <t>MFR-25FBF52-576K</t>
   </si>
 </sst>
 </file>
@@ -641,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,13 +688,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -690,25 +702,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="F2" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -716,7 +728,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -725,42 +737,42 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="F3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>93</v>
       </c>
       <c r="F4" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H4" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -771,22 +783,22 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" t="s">
         <v>8</v>
       </c>
-      <c r="F5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G5" t="s">
-        <v>9</v>
-      </c>
       <c r="H5" s="4" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -794,25 +806,25 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>95</v>
       </c>
       <c r="F6" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="G6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H6" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -820,22 +832,22 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
       <c r="E7" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F7" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="H7" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -843,22 +855,22 @@
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="F8" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H8" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -866,22 +878,22 @@
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="F9" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="H9" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -892,19 +904,19 @@
         <v>220</v>
       </c>
       <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
         <v>11</v>
       </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="F10" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="H10" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -915,19 +927,19 @@
         <v>68</v>
       </c>
       <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
         <v>11</v>
       </c>
-      <c r="D11" t="s">
-        <v>12</v>
-      </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="F11" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="H11" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -935,25 +947,25 @@
         <v>1</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H12" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -961,25 +973,25 @@
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
         <v>22</v>
       </c>
-      <c r="D13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" t="s">
-        <v>24</v>
-      </c>
       <c r="F13" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="G13" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -987,25 +999,25 @@
         <v>2</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
+        <v>96</v>
       </c>
       <c r="F14" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="G14" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H14" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1013,45 +1025,45 @@
         <v>1</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E15" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F15" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="G15" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E16" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F16" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G16" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1059,22 +1071,22 @@
         <v>1</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="F17" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="G17" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1082,22 +1094,22 @@
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>81</v>
+        <v>42</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="E18" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F18" t="s">
-        <v>81</v>
+        <v>42</v>
       </c>
       <c r="G18" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1105,22 +1117,22 @@
         <v>1</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C19" t="s">
-        <v>62</v>
+        <v>70</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="E19" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F19" t="s">
-        <v>78</v>
-      </c>
-      <c r="H19" t="s">
-        <v>83</v>
+        <v>70</v>
+      </c>
+      <c r="G19" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1128,22 +1140,22 @@
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="E20" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F20" t="s">
-        <v>77</v>
-      </c>
-      <c r="G20" t="s">
-        <v>40</v>
+        <v>67</v>
+      </c>
+      <c r="H20" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1151,52 +1163,75 @@
         <v>1</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="F21" t="s">
-        <v>67</v>
-      </c>
-      <c r="H21" t="s">
-        <v>68</v>
+        <v>66</v>
+      </c>
+      <c r="G21" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" t="s">
+        <v>57</v>
+      </c>
+      <c r="H22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>2</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" t="s">
-        <v>35</v>
-      </c>
-      <c r="F22" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F23" s="3"/>
+      <c r="B23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F26" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tweak TO220 packages and add board heatsink
</commit_message>
<xml_diff>
--- a/board/BOM.xlsx
+++ b/board/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="104">
   <si>
     <t>Qty</t>
   </si>
@@ -134,9 +134,6 @@
     <t>TO220BH</t>
   </si>
   <si>
-    <t>T1</t>
-  </si>
-  <si>
     <t>TRIAC</t>
   </si>
   <si>
@@ -278,12 +275,6 @@
     <t>SUP75P03-07-E3-H</t>
   </si>
   <si>
-    <t>560K</t>
-  </si>
-  <si>
-    <t>Need to experiment to find appropriate fuse type</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
@@ -321,6 +312,30 @@
   </si>
   <si>
     <t>MFR-25FBF52-576K</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>B3F-1020</t>
+  </si>
+  <si>
+    <t>S1, S2, S3, S4</t>
+  </si>
+  <si>
+    <t>TACTILE-SWITCH-6MM</t>
+  </si>
+  <si>
+    <t>SWITCH-MOMENTARY-6MM</t>
+  </si>
+  <si>
+    <t>Derated 25% per standard, consider fast-blow?</t>
+  </si>
+  <si>
+    <t>576K</t>
+  </si>
+  <si>
+    <t>version 3.0.1</t>
   </si>
 </sst>
 </file>
@@ -656,16 +671,16 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="24.85546875" customWidth="1"/>
     <col min="8" max="8" width="55.42578125" bestFit="1" customWidth="1"/>
@@ -688,13 +703,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -702,7 +717,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
@@ -711,16 +726,16 @@
         <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G2" t="s">
         <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -737,16 +752,16 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -763,16 +778,16 @@
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
       </c>
       <c r="H4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -789,16 +804,16 @@
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -806,7 +821,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
@@ -815,16 +830,16 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G6" t="s">
         <v>8</v>
       </c>
       <c r="H6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -832,7 +847,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -841,13 +856,13 @@
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -864,13 +879,13 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" t="s">
         <v>54</v>
-      </c>
-      <c r="H8" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -887,13 +902,13 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -910,13 +925,13 @@
         <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -933,13 +948,13 @@
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -959,13 +974,13 @@
         <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G12" t="s">
         <v>19</v>
       </c>
       <c r="H12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -985,13 +1000,13 @@
         <v>22</v>
       </c>
       <c r="F13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G13" t="s">
         <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -999,7 +1014,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -1008,16 +1023,16 @@
         <v>17</v>
       </c>
       <c r="E14" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G14" t="s">
         <v>19</v>
       </c>
       <c r="H14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1034,13 +1049,13 @@
         <v>35</v>
       </c>
       <c r="E15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" t="s">
         <v>36</v>
-      </c>
-      <c r="F15" t="s">
-        <v>53</v>
-      </c>
-      <c r="G15" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1048,22 +1063,22 @@
         <v>1</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
         <v>38</v>
-      </c>
-      <c r="C16" t="s">
-        <v>39</v>
       </c>
       <c r="D16" t="s">
         <v>35</v>
       </c>
       <c r="E16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" t="s">
         <v>40</v>
-      </c>
-      <c r="F16" t="s">
-        <v>38</v>
-      </c>
-      <c r="G16" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1071,22 +1086,22 @@
         <v>1</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" t="s">
         <v>82</v>
-      </c>
-      <c r="C17" t="s">
-        <v>83</v>
       </c>
       <c r="D17" t="s">
         <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="F17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1094,22 +1109,22 @@
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
         <v>42</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s">
         <v>43</v>
       </c>
-      <c r="D18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" t="s">
         <v>44</v>
-      </c>
-      <c r="F18" t="s">
-        <v>42</v>
-      </c>
-      <c r="G18" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1117,19 +1132,19 @@
         <v>1</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E19" t="s">
         <v>31</v>
       </c>
       <c r="F19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G19" t="s">
         <v>32</v>
@@ -1140,22 +1155,22 @@
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E20" t="s">
         <v>31</v>
       </c>
       <c r="F20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1163,7 +1178,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C21" t="s">
         <v>28</v>
@@ -1172,10 +1187,10 @@
         <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G21" t="s">
         <v>30</v>
@@ -1186,22 +1201,22 @@
         <v>1</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
         <v>26</v>
       </c>
       <c r="D22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E22" t="s">
         <v>27</v>
       </c>
       <c r="F22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H22" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1212,25 +1227,45 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" t="s">
         <v>58</v>
-      </c>
-      <c r="D23" t="s">
-        <v>59</v>
       </c>
       <c r="E23" t="s">
         <v>27</v>
       </c>
       <c r="F23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F24" s="3"/>
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" t="s">
+        <v>98</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="F26" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix the label order of caps
</commit_message>
<xml_diff>
--- a/board/BOM.xlsx
+++ b/board/BOM.xlsx
@@ -296,15 +296,6 @@
     <t>C8, C9</t>
   </si>
   <si>
-    <t>C4, C5, C10</t>
-  </si>
-  <si>
-    <t>C1, C2, C7</t>
-  </si>
-  <si>
-    <t>C3, C6</t>
-  </si>
-  <si>
     <t>D3, D4</t>
   </si>
   <si>
@@ -335,7 +326,16 @@
     <t>576K</t>
   </si>
   <si>
-    <t>version 3.0.1</t>
+    <t>C3, C4</t>
+  </si>
+  <si>
+    <t>C1, C2, C5</t>
+  </si>
+  <si>
+    <t>C6, C7, C10</t>
+  </si>
+  <si>
+    <t>version 3.0.2</t>
   </si>
 </sst>
 </file>
@@ -778,7 +778,7 @@
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="F4" t="s">
         <v>63</v>
@@ -787,7 +787,7 @@
         <v>8</v>
       </c>
       <c r="H4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -804,7 +804,7 @@
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="F5" t="s">
         <v>62</v>
@@ -830,7 +830,7 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="F6" t="s">
         <v>61</v>
@@ -847,7 +847,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -859,7 +859,7 @@
         <v>85</v>
       </c>
       <c r="F7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H7" t="s">
         <v>54</v>
@@ -1023,7 +1023,7 @@
         <v>17</v>
       </c>
       <c r="E14" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F14" t="s">
         <v>78</v>
@@ -1095,7 +1095,7 @@
         <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F17" t="s">
         <v>81</v>
@@ -1216,7 +1216,7 @@
         <v>56</v>
       </c>
       <c r="H22" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1244,19 +1244,19 @@
         <v>4</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D24" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E24" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
More adjustments to BOM and parts labels
</commit_message>
<xml_diff>
--- a/board/BOM.xlsx
+++ b/board/BOM.xlsx
@@ -119,9 +119,6 @@
     <t>Crystal Oscillator</t>
   </si>
   <si>
-    <t>U1</t>
-  </si>
-  <si>
     <t>8-bit Microcontroller with In-System Programmable Flash</t>
   </si>
   <si>
@@ -336,6 +333,9 @@
   </si>
   <si>
     <t>version 3.0.2</t>
+  </si>
+  <si>
+    <t>IC1</t>
   </si>
 </sst>
 </file>
@@ -671,7 +671,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,13 +703,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -717,7 +717,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
@@ -726,16 +726,16 @@
         <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G2" t="s">
         <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -752,16 +752,16 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -778,16 +778,16 @@
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
       </c>
       <c r="H4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -804,16 +804,16 @@
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -821,7 +821,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
@@ -830,16 +830,16 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G6" t="s">
         <v>8</v>
       </c>
       <c r="H6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -847,7 +847,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -856,13 +856,13 @@
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -879,13 +879,13 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" t="s">
         <v>53</v>
-      </c>
-      <c r="H8" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -902,13 +902,13 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -925,13 +925,13 @@
         <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -948,13 +948,13 @@
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -974,13 +974,13 @@
         <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G12" t="s">
         <v>19</v>
       </c>
       <c r="H12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1000,13 +1000,13 @@
         <v>22</v>
       </c>
       <c r="F13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G13" t="s">
         <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1014,7 +1014,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -1023,16 +1023,16 @@
         <v>17</v>
       </c>
       <c r="E14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G14" t="s">
         <v>19</v>
       </c>
       <c r="H14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1040,22 +1040,22 @@
         <v>1</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
         <v>33</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>34</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" t="s">
         <v>35</v>
-      </c>
-      <c r="E15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" t="s">
-        <v>52</v>
-      </c>
-      <c r="G15" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1063,22 +1063,22 @@
         <v>1</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
         <v>37</v>
       </c>
-      <c r="C16" t="s">
-        <v>38</v>
-      </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
         <v>29</v>
       </c>
       <c r="F16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1086,22 +1086,22 @@
         <v>1</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" t="s">
         <v>81</v>
       </c>
-      <c r="C17" t="s">
-        <v>82</v>
-      </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1109,22 +1109,22 @@
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
         <v>41</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" t="s">
         <v>42</v>
       </c>
-      <c r="D18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" t="s">
         <v>43</v>
-      </c>
-      <c r="F18" t="s">
-        <v>41</v>
-      </c>
-      <c r="G18" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1132,22 +1132,22 @@
         <v>1</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E19" t="s">
+        <v>103</v>
+      </c>
+      <c r="F19" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" t="s">
         <v>31</v>
-      </c>
-      <c r="F19" t="s">
-        <v>69</v>
-      </c>
-      <c r="G19" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1155,22 +1155,22 @@
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E20" t="s">
-        <v>31</v>
+        <v>103</v>
       </c>
       <c r="F20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1178,7 +1178,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C21" t="s">
         <v>28</v>
@@ -1187,10 +1187,10 @@
         <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G21" t="s">
         <v>30</v>
@@ -1201,22 +1201,22 @@
         <v>1</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
         <v>26</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E22" t="s">
         <v>27</v>
       </c>
       <c r="F22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1227,16 +1227,16 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" t="s">
         <v>57</v>
-      </c>
-      <c r="D23" t="s">
-        <v>58</v>
       </c>
       <c r="E23" t="s">
         <v>27</v>
       </c>
       <c r="F23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1244,19 +1244,19 @@
         <v>4</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1264,7 +1264,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F26" s="3"/>
     </row>

</xml_diff>

<commit_message>
Switched to 60V MOSFETs and updated BOM and inventory
</commit_message>
<xml_diff>
--- a/board/BOM.xlsx
+++ b/board/BOM.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="BOM" sheetId="1" r:id="rId1"/>
+    <sheet name="Inventory" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="101">
   <si>
     <t>Qty</t>
   </si>
@@ -113,9 +114,6 @@
     <t>CRYSTAL-V</t>
   </si>
   <si>
-    <t>Q2</t>
-  </si>
-  <si>
     <t>Crystal Oscillator</t>
   </si>
   <si>
@@ -134,12 +132,6 @@
     <t>TRIAC</t>
   </si>
   <si>
-    <t>IPP80P03P4L-04</t>
-  </si>
-  <si>
-    <t>IPP80P03P4L-04-H</t>
-  </si>
-  <si>
     <t>Q1</t>
   </si>
   <si>
@@ -266,12 +258,6 @@
     <t>Y1</t>
   </si>
   <si>
-    <t>SUP75P03-07-E3</t>
-  </si>
-  <si>
-    <t>SUP75P03-07-E3-H</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
@@ -302,9 +288,6 @@
     <t>MFR-25FBF52-576K</t>
   </si>
   <si>
-    <t>Q3</t>
-  </si>
-  <si>
     <t>B3F-1020</t>
   </si>
   <si>
@@ -332,17 +315,26 @@
     <t>C6, C7, C10</t>
   </si>
   <si>
-    <t>version 3.0.2</t>
-  </si>
-  <si>
     <t>IC1</t>
+  </si>
+  <si>
+    <t>SUP53P06-20-E3</t>
+  </si>
+  <si>
+    <t>Q2, Q3</t>
+  </si>
+  <si>
+    <t>version 3.1.1</t>
+  </si>
+  <si>
+    <t>Totals</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,6 +346,63 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -379,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -388,6 +437,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection sqref="A1:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,13 +759,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -717,7 +773,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
@@ -726,16 +782,16 @@
         <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G2" t="s">
         <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -752,16 +808,16 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -778,16 +834,16 @@
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
       </c>
       <c r="H4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -804,16 +860,16 @@
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -821,7 +877,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
@@ -830,16 +886,16 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="F6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G6" t="s">
         <v>8</v>
       </c>
       <c r="H6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -847,7 +903,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -856,13 +912,13 @@
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F7" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="H7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -879,13 +935,13 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -902,13 +958,13 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -925,13 +981,13 @@
         <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -948,13 +1004,13 @@
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -974,13 +1030,13 @@
         <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G12" t="s">
         <v>19</v>
       </c>
       <c r="H12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1000,13 +1056,13 @@
         <v>22</v>
       </c>
       <c r="F13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G13" t="s">
         <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1014,7 +1070,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -1023,16 +1079,16 @@
         <v>17</v>
       </c>
       <c r="E14" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G14" t="s">
         <v>19</v>
       </c>
       <c r="H14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1040,45 +1096,45 @@
         <v>1</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
         <v>32</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>33</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" t="s">
         <v>34</v>
-      </c>
-      <c r="E15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" t="s">
-        <v>51</v>
-      </c>
-      <c r="G15" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F16" t="s">
+        <v>97</v>
+      </c>
+      <c r="G16" t="s">
         <v>36</v>
-      </c>
-      <c r="C16" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1086,22 +1142,22 @@
         <v>1</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>80</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>81</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E17" t="s">
-        <v>92</v>
+        <v>39</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
+        <v>37</v>
       </c>
       <c r="G17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1109,22 +1165,22 @@
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" t="s">
-        <v>41</v>
+        <v>65</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="F18" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="G18" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1132,22 +1188,22 @@
         <v>1</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
+      </c>
+      <c r="C19" t="s">
+        <v>47</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E19" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="F19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G19" t="s">
-        <v>31</v>
+        <v>62</v>
+      </c>
+      <c r="H19" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1155,22 +1211,22 @@
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="D20" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="E20" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="F20" t="s">
-        <v>65</v>
-      </c>
-      <c r="H20" t="s">
-        <v>70</v>
+        <v>61</v>
+      </c>
+      <c r="G20" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1178,36 +1234,36 @@
         <v>1</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="E21" t="s">
-        <v>79</v>
+        <v>27</v>
       </c>
       <c r="F21" t="s">
-        <v>64</v>
-      </c>
-      <c r="G21" t="s">
-        <v>30</v>
+        <v>52</v>
+      </c>
+      <c r="H21" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="D22" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="E22" t="s">
         <v>27</v>
@@ -1215,61 +1271,592 @@
       <c r="F22" t="s">
         <v>55</v>
       </c>
-      <c r="H22" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" t="s">
-        <v>56</v>
+        <v>90</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>89</v>
       </c>
       <c r="E23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F23" t="s">
-        <v>58</v>
+        <v>88</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>4</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D24" t="s">
-        <v>95</v>
-      </c>
-      <c r="E24" t="s">
-        <v>94</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>93</v>
-      </c>
+      <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="F26" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="12"/>
+    <col min="4" max="4" width="9.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="9">
+        <v>42215</v>
+      </c>
+      <c r="E1" s="10">
+        <v>10</v>
+      </c>
+      <c r="F1" s="9">
+        <v>42304</v>
+      </c>
+      <c r="G1" s="10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="12">
+        <f>SUM(D2:ZZ2)</f>
+        <v>20</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6">
+        <v>60</v>
+      </c>
+      <c r="G2" s="7">
+        <f>-(G$1*$A2)</f>
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="12">
+        <f>SUM(D3:ZZ3)</f>
+        <v>170</v>
+      </c>
+      <c r="D3" s="6">
+        <v>200</v>
+      </c>
+      <c r="E3" s="7">
+        <f>-(E$1*$A3)</f>
+        <v>-10</v>
+      </c>
+      <c r="G3" s="7">
+        <f>-(G$1*$A3)</f>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="12">
+        <f t="shared" ref="C4:C22" si="0">SUM(D4:ZZ4)</f>
+        <v>40</v>
+      </c>
+      <c r="D4" s="6">
+        <v>100</v>
+      </c>
+      <c r="E4" s="7">
+        <f t="shared" ref="E4:E22" si="1">-(E$1*$A4)</f>
+        <v>-20</v>
+      </c>
+      <c r="G4" s="7">
+        <f>-(G$1*$A4)</f>
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>10</v>
+      </c>
+      <c r="E5" s="7">
+        <f t="shared" si="1"/>
+        <v>-10</v>
+      </c>
+      <c r="F5" s="6">
+        <v>20</v>
+      </c>
+      <c r="G5" s="7">
+        <f t="shared" ref="G5:G22" si="2">-(G$1*$A5)</f>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="12">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D6" s="6">
+        <v>100</v>
+      </c>
+      <c r="E6" s="7">
+        <f t="shared" si="1"/>
+        <v>-20</v>
+      </c>
+      <c r="G6" s="7">
+        <f t="shared" si="2"/>
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="12">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="D7" s="6">
+        <v>100</v>
+      </c>
+      <c r="E7" s="7">
+        <f t="shared" si="1"/>
+        <v>-10</v>
+      </c>
+      <c r="G7" s="7">
+        <f t="shared" si="2"/>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D8" s="6">
+        <v>10</v>
+      </c>
+      <c r="E8" s="7">
+        <f t="shared" si="1"/>
+        <v>-10</v>
+      </c>
+      <c r="F8" s="6">
+        <v>20</v>
+      </c>
+      <c r="G8" s="7">
+        <f t="shared" si="2"/>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="6">
+        <v>10</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" si="1"/>
+        <v>-10</v>
+      </c>
+      <c r="F9" s="6">
+        <v>20</v>
+      </c>
+      <c r="G9" s="7">
+        <f t="shared" si="2"/>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="6">
+        <v>10</v>
+      </c>
+      <c r="E10" s="7">
+        <f t="shared" si="1"/>
+        <v>-10</v>
+      </c>
+      <c r="F10" s="6">
+        <v>20</v>
+      </c>
+      <c r="G10" s="7">
+        <f t="shared" si="2"/>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D11" s="6">
+        <v>100</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="1"/>
+        <v>-30</v>
+      </c>
+      <c r="G11" s="7">
+        <f t="shared" si="2"/>
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D12" s="6">
+        <v>100</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" si="1"/>
+        <v>-30</v>
+      </c>
+      <c r="G12" s="7">
+        <f t="shared" si="2"/>
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="12">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D13" s="6">
+        <v>100</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="1"/>
+        <v>-20</v>
+      </c>
+      <c r="G13" s="7">
+        <f t="shared" si="2"/>
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D14" s="6">
+        <v>20</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" si="1"/>
+        <v>-20</v>
+      </c>
+      <c r="F14" s="6">
+        <v>40</v>
+      </c>
+      <c r="G14" s="7">
+        <f t="shared" si="2"/>
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D15" s="6">
+        <v>10</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" si="1"/>
+        <v>-10</v>
+      </c>
+      <c r="F15" s="6">
+        <v>20</v>
+      </c>
+      <c r="G15" s="7">
+        <f t="shared" si="2"/>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D16" s="6">
+        <v>10</v>
+      </c>
+      <c r="E16" s="7">
+        <f t="shared" si="1"/>
+        <v>-10</v>
+      </c>
+      <c r="F16" s="6">
+        <v>20</v>
+      </c>
+      <c r="G16" s="7">
+        <f t="shared" si="2"/>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="12">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="D17" s="6">
+        <v>200</v>
+      </c>
+      <c r="E17" s="7">
+        <f t="shared" si="1"/>
+        <v>-20</v>
+      </c>
+      <c r="G17" s="7">
+        <f t="shared" si="2"/>
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="12">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="D18" s="6">
+        <v>200</v>
+      </c>
+      <c r="E18" s="7">
+        <f t="shared" si="1"/>
+        <v>-20</v>
+      </c>
+      <c r="G18" s="7">
+        <f t="shared" si="2"/>
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D19" s="6">
+        <v>10</v>
+      </c>
+      <c r="E19" s="7">
+        <f t="shared" si="1"/>
+        <v>-10</v>
+      </c>
+      <c r="F19" s="6">
+        <v>20</v>
+      </c>
+      <c r="G19" s="7">
+        <f t="shared" si="2"/>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="12">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="D20" s="6">
+        <v>100</v>
+      </c>
+      <c r="E20" s="7">
+        <f t="shared" si="1"/>
+        <v>-10</v>
+      </c>
+      <c r="G20" s="7">
+        <f t="shared" si="2"/>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="12">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="D21" s="6">
+        <v>100</v>
+      </c>
+      <c r="E21" s="7">
+        <f t="shared" si="1"/>
+        <v>-10</v>
+      </c>
+      <c r="G21" s="7">
+        <f t="shared" si="2"/>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="12">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D22" s="6">
+        <v>100</v>
+      </c>
+      <c r="E22" s="7">
+        <f t="shared" si="1"/>
+        <v>-20</v>
+      </c>
+      <c r="G22" s="7">
+        <f t="shared" si="2"/>
+        <v>-40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update BOM and test procedures
</commit_message>
<xml_diff>
--- a/board/BOM.xlsx
+++ b/board/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SaintGimp\MotorController\board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263659E4-6118-49B0-9811-103FA1CCCAF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A044D687-59A6-4C5A-90F9-46563D613FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5310" yWindow="4650" windowWidth="23025" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="133">
   <si>
     <t>Qty</t>
   </si>
@@ -432,6 +432,9 @@
   </si>
   <si>
     <t>20pF capacitor</t>
+  </si>
+  <si>
+    <t>7805SRH-C</t>
   </si>
 </sst>
 </file>
@@ -1464,7 +1467,7 @@
   <dimension ref="A1:T25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2493,6 +2496,9 @@
       <c r="C16" t="s">
         <v>37</v>
       </c>
+      <c r="D16" t="s">
+        <v>132</v>
+      </c>
       <c r="E16" s="12">
         <f t="shared" si="0"/>
         <v>60</v>

</xml_diff>